<commit_message>
programa de caras de dado
</commit_message>
<xml_diff>
--- a/resultados.xlsx
+++ b/resultados.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -489,6 +489,19 @@
         <v>88</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Fransisco</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>35</v>
+      </c>
+      <c r="C5" t="n">
+        <v>88</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>